<commit_message>
Updating to color figures
</commit_message>
<xml_diff>
--- a/Spreadsheets/PredictionResults.xlsx
+++ b/Spreadsheets/PredictionResults.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\EmailPaper\Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kstraub/Documents/Research/EmailPaper/EmailPaper/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prediction Results" sheetId="1" r:id="rId1"/>
     <sheet name="Split Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -140,7 +143,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="tx1"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -181,22 +184,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -218,7 +221,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -259,22 +262,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -290,11 +293,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="71629552"/>
-        <c:axId val="259980816"/>
+        <c:axId val="-2130580400"/>
+        <c:axId val="-2127374064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71629552"/>
+        <c:axId val="-2130580400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -337,7 +340,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259980816"/>
+        <c:crossAx val="-2127374064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -345,7 +348,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="259980816"/>
+        <c:axId val="-2127374064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +455,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71629552"/>
+        <c:crossAx val="-2130580400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1159,9 +1162,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1194,9 +1197,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1379,16 +1382,16 @@
   <dimension ref="A2:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1431,7 +1434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1466,7 +1469,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>